<commit_message>
LOI Category processing updated
</commit_message>
<xml_diff>
--- a/data/outputs/HWW AUD Data Requirement.xlsx
+++ b/data/outputs/HWW AUD Data Requirement.xlsx
@@ -671,7 +671,11 @@
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R2" t="inlineStr">
         <is>
           <t>No</t>
@@ -757,7 +761,11 @@
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R3" t="inlineStr">
         <is>
           <t>No</t>
@@ -4495,7 +4503,11 @@
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R32" t="inlineStr">
         <is>
           <t>No</t>
@@ -4573,7 +4585,11 @@
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R33" t="inlineStr">
         <is>
           <t>No</t>
@@ -5571,7 +5587,11 @@
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
-      <c r="Q41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R41" t="inlineStr">
         <is>
           <t>No</t>
@@ -6421,7 +6441,11 @@
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
-      <c r="Q48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R48" t="inlineStr">
         <is>
           <t>No</t>
@@ -7003,7 +7027,11 @@
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R53" t="inlineStr">
         <is>
           <t>No</t>
@@ -7317,7 +7345,11 @@
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R56" t="inlineStr">
         <is>
           <t>No</t>
@@ -7523,7 +7555,11 @@
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr"/>
-      <c r="Q58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R58" t="inlineStr">
         <is>
           <t>No</t>
@@ -7605,7 +7641,11 @@
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr"/>
-      <c r="Q59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R59" t="inlineStr">
         <is>
           <t>No</t>
@@ -10291,7 +10331,11 @@
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr"/>
       <c r="P81" t="inlineStr"/>
-      <c r="Q81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R81" t="inlineStr">
         <is>
           <t>No</t>
@@ -10493,7 +10537,11 @@
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
       <c r="P83" t="inlineStr"/>
-      <c r="Q83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R83" t="inlineStr">
         <is>
           <t>No</t>
@@ -12223,7 +12271,11 @@
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr"/>
       <c r="P97" t="inlineStr"/>
-      <c r="Q97" t="inlineStr"/>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R97" t="inlineStr">
         <is>
           <t>No</t>
@@ -13373,7 +13425,11 @@
       <c r="N106" t="inlineStr"/>
       <c r="O106" t="inlineStr"/>
       <c r="P106" t="inlineStr"/>
-      <c r="Q106" t="inlineStr"/>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R106" t="inlineStr">
         <is>
           <t>No</t>
@@ -15139,7 +15195,11 @@
       <c r="N120" t="inlineStr"/>
       <c r="O120" t="inlineStr"/>
       <c r="P120" t="inlineStr"/>
-      <c r="Q120" t="inlineStr"/>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R120" t="inlineStr">
         <is>
           <t>No</t>
@@ -16089,7 +16149,11 @@
       <c r="N128" t="inlineStr"/>
       <c r="O128" t="inlineStr"/>
       <c r="P128" t="inlineStr"/>
-      <c r="Q128" t="inlineStr"/>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R128" t="inlineStr">
         <is>
           <t>No</t>
@@ -16299,7 +16363,11 @@
       <c r="N130" t="inlineStr"/>
       <c r="O130" t="inlineStr"/>
       <c r="P130" t="inlineStr"/>
-      <c r="Q130" t="inlineStr"/>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R130" t="inlineStr">
         <is>
           <t>No</t>
@@ -16373,7 +16441,11 @@
       <c r="N131" t="inlineStr"/>
       <c r="O131" t="inlineStr"/>
       <c r="P131" t="inlineStr"/>
-      <c r="Q131" t="inlineStr"/>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R131" t="inlineStr">
         <is>
           <t>No</t>
@@ -17111,7 +17183,11 @@
       <c r="N137" t="inlineStr"/>
       <c r="O137" t="inlineStr"/>
       <c r="P137" t="inlineStr"/>
-      <c r="Q137" t="inlineStr"/>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R137" t="inlineStr">
         <is>
           <t>No</t>
@@ -17725,7 +17801,11 @@
       <c r="N142" t="inlineStr"/>
       <c r="O142" t="inlineStr"/>
       <c r="P142" t="inlineStr"/>
-      <c r="Q142" t="inlineStr"/>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R142" t="inlineStr">
         <is>
           <t>No</t>
@@ -18051,7 +18131,11 @@
       <c r="N145" t="inlineStr"/>
       <c r="O145" t="inlineStr"/>
       <c r="P145" t="inlineStr"/>
-      <c r="Q145" t="inlineStr"/>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R145" t="inlineStr">
         <is>
           <t>No</t>
@@ -18259,7 +18343,11 @@
       <c r="N147" t="inlineStr"/>
       <c r="O147" t="inlineStr"/>
       <c r="P147" t="inlineStr"/>
-      <c r="Q147" t="inlineStr"/>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R147" t="inlineStr">
         <is>
           <t>No</t>
@@ -18477,7 +18565,11 @@
       <c r="N149" t="inlineStr"/>
       <c r="O149" t="inlineStr"/>
       <c r="P149" t="inlineStr"/>
-      <c r="Q149" t="inlineStr"/>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R149" t="inlineStr">
         <is>
           <t>No</t>
@@ -18547,7 +18639,11 @@
       <c r="N150" t="inlineStr"/>
       <c r="O150" t="inlineStr"/>
       <c r="P150" t="inlineStr"/>
-      <c r="Q150" t="inlineStr"/>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R150" t="inlineStr">
         <is>
           <t>No</t>
@@ -20533,7 +20629,11 @@
       <c r="N166" t="inlineStr"/>
       <c r="O166" t="inlineStr"/>
       <c r="P166" t="inlineStr"/>
-      <c r="Q166" t="inlineStr"/>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R166" t="inlineStr">
         <is>
           <t>No</t>
@@ -20615,7 +20715,11 @@
       <c r="N167" t="inlineStr"/>
       <c r="O167" t="inlineStr"/>
       <c r="P167" t="inlineStr"/>
-      <c r="Q167" t="inlineStr"/>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R167" t="inlineStr">
         <is>
           <t>No</t>
@@ -23025,7 +23129,11 @@
       <c r="N186" t="inlineStr"/>
       <c r="O186" t="inlineStr"/>
       <c r="P186" t="inlineStr"/>
-      <c r="Q186" t="inlineStr"/>
+      <c r="Q186" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R186" t="inlineStr">
         <is>
           <t>No</t>
@@ -23863,7 +23971,11 @@
       <c r="N193" t="inlineStr"/>
       <c r="O193" t="inlineStr"/>
       <c r="P193" t="inlineStr"/>
-      <c r="Q193" t="inlineStr"/>
+      <c r="Q193" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R193" t="inlineStr">
         <is>
           <t>No</t>
@@ -24205,7 +24317,11 @@
       <c r="N196" t="inlineStr"/>
       <c r="O196" t="inlineStr"/>
       <c r="P196" t="inlineStr"/>
-      <c r="Q196" t="inlineStr"/>
+      <c r="Q196" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R196" t="inlineStr">
         <is>
           <t>No</t>
@@ -24425,7 +24541,11 @@
       <c r="N198" t="inlineStr"/>
       <c r="O198" t="inlineStr"/>
       <c r="P198" t="inlineStr"/>
-      <c r="Q198" t="inlineStr"/>
+      <c r="Q198" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R198" t="inlineStr">
         <is>
           <t>No</t>
@@ -24739,7 +24859,11 @@
       <c r="N201" t="inlineStr"/>
       <c r="O201" t="inlineStr"/>
       <c r="P201" t="inlineStr"/>
-      <c r="Q201" t="inlineStr"/>
+      <c r="Q201" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R201" t="inlineStr">
         <is>
           <t>No</t>
@@ -24817,7 +24941,11 @@
       <c r="N202" t="inlineStr"/>
       <c r="O202" t="inlineStr"/>
       <c r="P202" t="inlineStr"/>
-      <c r="Q202" t="inlineStr"/>
+      <c r="Q202" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R202" t="inlineStr">
         <is>
           <t>No</t>
@@ -26059,7 +26187,11 @@
       <c r="N212" t="inlineStr"/>
       <c r="O212" t="inlineStr"/>
       <c r="P212" t="inlineStr"/>
-      <c r="Q212" t="inlineStr"/>
+      <c r="Q212" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R212" t="inlineStr">
         <is>
           <t>No</t>
@@ -26265,7 +26397,11 @@
       <c r="N214" t="inlineStr"/>
       <c r="O214" t="inlineStr"/>
       <c r="P214" t="inlineStr"/>
-      <c r="Q214" t="inlineStr"/>
+      <c r="Q214" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R214" t="inlineStr">
         <is>
           <t>No</t>
@@ -26343,7 +26479,11 @@
       <c r="N215" t="inlineStr"/>
       <c r="O215" t="inlineStr"/>
       <c r="P215" t="inlineStr"/>
-      <c r="Q215" t="inlineStr"/>
+      <c r="Q215" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R215" t="inlineStr">
         <is>
           <t>No</t>
@@ -27189,7 +27329,11 @@
       <c r="N222" t="inlineStr"/>
       <c r="O222" t="inlineStr"/>
       <c r="P222" t="inlineStr"/>
-      <c r="Q222" t="inlineStr"/>
+      <c r="Q222" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R222" t="inlineStr">
         <is>
           <t>No</t>
@@ -27527,7 +27671,11 @@
       <c r="N225" t="inlineStr"/>
       <c r="O225" t="inlineStr"/>
       <c r="P225" t="inlineStr"/>
-      <c r="Q225" t="inlineStr"/>
+      <c r="Q225" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R225" t="inlineStr">
         <is>
           <t>No</t>
@@ -27605,7 +27753,11 @@
       <c r="N226" t="inlineStr"/>
       <c r="O226" t="inlineStr"/>
       <c r="P226" t="inlineStr"/>
-      <c r="Q226" t="inlineStr"/>
+      <c r="Q226" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R226" t="inlineStr">
         <is>
           <t>No</t>
@@ -29299,7 +29451,11 @@
       <c r="N240" t="inlineStr"/>
       <c r="O240" t="inlineStr"/>
       <c r="P240" t="inlineStr"/>
-      <c r="Q240" t="inlineStr"/>
+      <c r="Q240" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R240" t="inlineStr">
         <is>
           <t>No</t>
@@ -29489,7 +29645,11 @@
       <c r="N242" t="inlineStr"/>
       <c r="O242" t="inlineStr"/>
       <c r="P242" t="inlineStr"/>
-      <c r="Q242" t="inlineStr"/>
+      <c r="Q242" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R242" t="inlineStr">
         <is>
           <t>No</t>
@@ -29671,7 +29831,11 @@
       <c r="N244" t="inlineStr"/>
       <c r="O244" t="inlineStr"/>
       <c r="P244" t="inlineStr"/>
-      <c r="Q244" t="inlineStr"/>
+      <c r="Q244" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R244" t="inlineStr">
         <is>
           <t>No</t>
@@ -33289,7 +33453,11 @@
       <c r="N275" t="inlineStr"/>
       <c r="O275" t="inlineStr"/>
       <c r="P275" t="inlineStr"/>
-      <c r="Q275" t="inlineStr"/>
+      <c r="Q275" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="R275" t="inlineStr">
         <is>
           <t>No</t>

</xml_diff>